<commit_message>
Updated the test excel sheet.
</commit_message>
<xml_diff>
--- a/PandaTrials/majorLazor.xlsx
+++ b/PandaTrials/majorLazor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gouthamr/Documents/PythonProjects/PandaTrials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540C17C1-A504-F542-9D3B-64FA90D0AC18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8F8DBB-B22A-784D-8405-480EFC4A9B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{610B568E-8043-1049-896E-8969EA46D4E1}"/>
+    <workbookView xWindow="7800" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{610B568E-8043-1049-896E-8969EA46D4E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,38 +296,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,7 +647,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,122 +675,122 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+      <c r="A3" s="12">
         <v>2012</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>2013</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="1"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
+      <c r="A12" s="13">
         <v>2014</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
+      <c r="A16" s="13">
         <v>2015</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -810,17 +810,17 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
+      <c r="A18" s="13">
         <v>2016</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -832,7 +832,7 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
         <v>22</v>
       </c>
@@ -848,65 +848,65 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A22" s="15">
+      <c r="A22" s="13">
         <v>2017</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A24" s="15">
+      <c r="A24" s="13">
         <v>2018</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -916,7 +916,7 @@
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="15">
+      <c r="A28" s="13">
         <v>2019</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -926,21 +926,21 @@
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="1"/>

</xml_diff>

<commit_message>
loc and iloc demos added.
</commit_message>
<xml_diff>
--- a/PandaTrials/majorLazor.xlsx
+++ b/PandaTrials/majorLazor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gouthamr/Documents/PythonProjects/PandaTrials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8F8DBB-B22A-784D-8405-480EFC4A9B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4841E9B-8116-6241-B763-CC7F70E584BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{610B568E-8043-1049-896E-8969EA46D4E1}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>